<commit_message>
aggiornamento Matrice delle Resp.
</commit_message>
<xml_diff>
--- a/Progettazione/Org_Resp.xlsx
+++ b/Progettazione/Org_Resp.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATURITA\ProgettoMaturita_FrigoAutomatico\Progettazione\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1185" tabRatio="176"/>
   </bookViews>
@@ -76,9 +81,6 @@
     <t>WAR</t>
   </si>
   <si>
-    <t>Casi d' uso</t>
-  </si>
-  <si>
     <t>PERT/GANT</t>
   </si>
   <si>
@@ -122,13 +124,16 @@
   </si>
   <si>
     <t>Costruzione Frigo</t>
+  </si>
+  <si>
+    <t>Depliant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,37 +493,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -527,10 +544,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,18 +556,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -569,6 +574,9 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,9 +602,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -605,6 +610,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -863,21 +876,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
@@ -891,7 +904,7 @@
     <col min="30" max="30" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="19.5" thickBot="1">
+    <row r="1" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,19 +912,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:23" ht="19.5" thickBot="1">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1"/>
-    <row r="5" spans="1:23" ht="19.5" thickBot="1">
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -919,25 +932,25 @@
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="7" spans="1:23" ht="19.5" thickBot="1">
+    <row r="7" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="11"/>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50"/>
-      <c r="I7" s="44" t="s">
+      <c r="F7" s="50"/>
+      <c r="G7" s="51"/>
+      <c r="I7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
       <c r="W7" s="12"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1">
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>5</v>
       </c>
@@ -959,15 +972,15 @@
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L8" s="16"/>
       <c r="M8" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N8" s="16"/>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>8</v>
       </c>
@@ -976,71 +989,71 @@
       <c r="D9" s="41"/>
       <c r="E9" s="40"/>
       <c r="F9" s="40"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="37" t="s">
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
       <c r="V10" s="12"/>
     </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
     </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
     </row>
-    <row r="17" spans="1:30" ht="19.5" thickBot="1">
+    <row r="17" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1049,29 +1062,29 @@
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="G17" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="J17" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="43"/>
-      <c r="J17" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="52"/>
-    </row>
-    <row r="18" spans="1:30" ht="15.75" thickBot="1">
+      <c r="K17" s="53"/>
+    </row>
+    <row r="18" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="39"/>
       <c r="C18" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="15" t="s">
@@ -1083,7 +1096,7 @@
       </c>
       <c r="L18" s="16"/>
       <c r="M18" s="15" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="N18" s="16"/>
       <c r="O18" s="15" t="s">
@@ -1095,183 +1108,183 @@
       </c>
       <c r="R18" s="16"/>
       <c r="S18" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V18" s="16"/>
       <c r="W18" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X18" s="16"/>
-      <c r="Y18" s="21" t="s">
+      <c r="Y18" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB18" s="31"/>
+      <c r="AB18" s="22"/>
       <c r="AC18" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD18" s="16"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="40"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="41"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="27"/>
-    </row>
-    <row r="20" spans="1:30">
-      <c r="A20" s="37" t="s">
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="18"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="17"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
       <c r="AA20" s="25"/>
       <c r="AB20" s="25"/>
-      <c r="AC20" s="17"/>
-      <c r="AD20" s="18"/>
-    </row>
-    <row r="21" spans="1:30">
-      <c r="A21" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="17"/>
-      <c r="X21" s="18"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="20"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="20"/>
       <c r="Y21" s="25"/>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25"/>
       <c r="AB21" s="25"/>
-      <c r="AC21" s="17"/>
-      <c r="AD21" s="18"/>
-    </row>
-    <row r="22" spans="1:30">
-      <c r="A22" s="37" t="s">
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="20"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="18"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="20"/>
       <c r="Y22" s="25"/>
       <c r="Z22" s="25"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="18"/>
-    </row>
-    <row r="28" spans="1:30">
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="20"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C28" s="14"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C29" s="14"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -1280,7 +1293,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -1289,7 +1302,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1298,7 +1311,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -1307,7 +1320,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -1316,7 +1329,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -1325,7 +1338,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -1334,7 +1347,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1343,7 +1356,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -1352,7 +1365,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -1361,7 +1374,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -1370,7 +1383,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -1379,7 +1392,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -1388,7 +1401,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -1397,7 +1410,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -1406,7 +1419,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -1415,7 +1428,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -1424,7 +1437,7 @@
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -1433,13 +1446,13 @@
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -1448,7 +1461,7 @@
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -1457,7 +1470,7 @@
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -1466,7 +1479,7 @@
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -1475,7 +1488,7 @@
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -1484,7 +1497,7 @@
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -1493,7 +1506,7 @@
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -1502,7 +1515,7 @@
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
@@ -1511,7 +1524,7 @@
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
       <c r="C59" s="14"/>
@@ -1520,7 +1533,7 @@
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -1529,7 +1542,7 @@
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
@@ -1538,7 +1551,7 @@
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
       <c r="C62" s="14"/>
@@ -1547,14 +1560,13 @@
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="I10:J10"/>
@@ -1567,9 +1579,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="I8:J8"/>
@@ -1580,8 +1589,7 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="K8:L8"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="A9:B9"/>
@@ -1590,7 +1598,9 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="M20:N20"/>
@@ -1600,7 +1610,6 @@
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="O18:P18"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1610,21 +1619,8 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A21:B21"/>
@@ -1637,7 +1633,13 @@
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="S21:T21"/>
     <mergeCell ref="S22:T22"/>
-    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
     <mergeCell ref="AA22:AB22"/>
     <mergeCell ref="Y22:Z22"/>
     <mergeCell ref="Y21:Z21"/>
@@ -1646,6 +1648,15 @@
     <mergeCell ref="AC22:AD22"/>
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="S19:T19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="AC18:AD18"/>
     <mergeCell ref="AC19:AD19"/>
     <mergeCell ref="AC20:AD20"/>
@@ -1668,6 +1679,8 @@
     <mergeCell ref="U18:V18"/>
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="S20:T20"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="Q18:R18"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>